<commit_message>
Commiting changes for CCDI test cases failed in jenkins
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002371_Sex-Male_DiagAnatomicsite-C42.0Blood.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002371_Sex-Male_DiagAnatomicsite-C42.0Blood.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\04-29-25\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\05-01-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBC928F-B11F-4501-9E63-375C40FDB0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B618C6E6-E35E-4B6B-949B-EAF46EF96DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -163,28 +163,6 @@
     df_sequencing_file seq ON smp.id = seq."sample.id"
 WHERE 
     std.dbgap_accession = 'phs002371';</t>
-  </si>
-  <si>
-    <t>SELECT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    Null  AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs002371' 
-    AND prt.sex_at_birth = 'Male'
-	and dgn.anatomic_site= 'C42.0 : Blood'
-ORDER BY 
-    smp.sample_id ASC;</t>
   </si>
   <si>
     <t>WITH file_data AS (
@@ -250,6 +228,31 @@
 ORDER BY  
     fd.file_name
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    smp.sample_id AS "Sample ID",
+    prt.participant_id AS "Participant ID",
+    std.dbgap_accession AS "Study ID",
+    smp.anatomic_site AS "Sample Anatomic Site",
+    COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
+    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
+    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
+    Null  AS "Sample Diagnosis"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+WHERE 
+    std.dbgap_accession = 'phs002371' 
+    AND prt.sex_at_birth = 'Male'
+	and dgn.anatomic_site= 'C42.0 : Blood'
+ORDER BY 
+    smp.sample_id ASC;</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,12 +709,12 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="393.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -720,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>

</xml_diff>